<commit_message>
boolean for unmoderated testing platform
</commit_message>
<xml_diff>
--- a/public/users/imports/Wrapt User Import Template.xlsx
+++ b/public/users/imports/Wrapt User Import Template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
     <t>first_name</t>
   </si>
@@ -20,6 +20,9 @@
   </si>
   <si>
     <t>email</t>
+  </si>
+  <si>
+    <t>unmoderated_testing_platform</t>
   </si>
 </sst>
 </file>
@@ -89,7 +92,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -99,10 +102,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -261,13 +261,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -366,10 +360,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -624,13 +618,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -943,10 +931,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1209,7 +1197,7 @@
     <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6719" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.1719" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.1719" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.5" style="1" customWidth="1"/>
@@ -1233,7 +1221,9 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -1246,148 +1236,148 @@
       <c r="N1" s="3"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>